<commit_message>
Adding taxa-specific biomass spectra
</commit_message>
<xml_diff>
--- a/ancillary/plankton_annotated_taxonomy.xlsx
+++ b/ancillary/plankton_annotated_taxonomy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dugennem/GIT/PSSdb/ancillary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BED0FA4-9A49-ED42-8E85-BB526B6B6B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFF81FB-F044-424B-8CC1-8A800B88DFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-1100" windowWidth="38400" windowHeight="17840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17664,10 +17664,10 @@
   <dimension ref="A1:T1282"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="R29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S1283" sqref="S1283"/>
+      <selection pane="bottomRight" activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix for linear fit performed on one row dataframe with na. Testing on all datasets
</commit_message>
<xml_diff>
--- a/ancillary/plankton_annotated_taxonomy.xlsx
+++ b/ancillary/plankton_annotated_taxonomy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dugennem/GIT/PSSdb/ancillary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFF81FB-F044-424B-8CC1-8A800B88DFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790769B4-20C7-F249-A772-683FEB88B7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-1100" windowWidth="38400" windowHeight="17840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17664,10 +17664,10 @@
   <dimension ref="A1:T1282"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="R29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="R477" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T29" sqref="T29"/>
+      <selection pane="bottomRight" activeCell="S477" sqref="S477:S951"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -35305,7 +35305,7 @@
         <v>1899</v>
       </c>
       <c r="S315" t="s">
-        <v>1894</v>
+        <v>140</v>
       </c>
       <c r="T315" t="s">
         <v>87</v>
@@ -35358,7 +35358,7 @@
         <v>1904</v>
       </c>
       <c r="S316" t="s">
-        <v>1894</v>
+        <v>140</v>
       </c>
       <c r="T316" t="s">
         <v>87</v>
@@ -44497,7 +44497,7 @@
         <v>2918</v>
       </c>
       <c r="S477" t="s">
-        <v>1894</v>
+        <v>140</v>
       </c>
       <c r="T477" t="s">
         <v>87</v>
@@ -62157,7 +62157,7 @@
         <v>1904</v>
       </c>
       <c r="S790" t="s">
-        <v>1894</v>
+        <v>140</v>
       </c>
       <c r="T790" t="s">
         <v>87</v>
@@ -62210,7 +62210,7 @@
         <v>1904</v>
       </c>
       <c r="S791" t="s">
-        <v>1894</v>
+        <v>140</v>
       </c>
       <c r="T791" t="s">
         <v>87</v>
@@ -66062,7 +66062,7 @@
         <v>1904</v>
       </c>
       <c r="S872" t="s">
-        <v>1894</v>
+        <v>140</v>
       </c>
       <c r="T872" t="s">
         <v>87</v>
@@ -70033,7 +70033,7 @@
         <v>1904</v>
       </c>
       <c r="S951" t="s">
-        <v>1894</v>
+        <v>140</v>
       </c>
       <c r="T951" t="s">
         <v>87</v>

</xml_diff>